<commit_message>
stuck at encoding balance
</commit_message>
<xml_diff>
--- a/sofaaudit/input.orig.small.xlsx
+++ b/sofaaudit/input.orig.small.xlsx
@@ -11781,9 +11781,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11949,7 +11951,7 @@
     <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="48">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -11973,6 +11975,7 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -11995,6 +11998,7 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -41665,7 +41669,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -41732,20 +41736,20 @@
         <v>560</v>
       </c>
       <c r="G2" s="74">
-        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B2,Encoding!C:C,C2,Encoding!B:B,'RESULT BALANCE'!D2)</f>
-        <v>-520</v>
+        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B2,Encoding!C:C,C2)</f>
+        <v>-530</v>
       </c>
       <c r="H2" s="80">
         <f>G2+F2</f>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I2" s="67">
         <f>IF(H2&gt;0,H2,0)</f>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="J2" s="71">
         <f>I2</f>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="K2" s="67" t="s">
         <v>3655</v>
@@ -41792,16 +41796,16 @@
         <v>655.14567999999997</v>
       </c>
       <c r="G3" s="74">
-        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B3,Encoding!C:C,C3,Encoding!B:B,'RESULT BALANCE'!D3)</f>
-        <v>-520</v>
+        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B3,Encoding!C:C,C3)</f>
+        <v>-530</v>
       </c>
       <c r="H3" s="80">
         <f t="shared" ref="H3:H7" si="0">G3+F3</f>
-        <v>135.14567999999997</v>
+        <v>125.14567999999997</v>
       </c>
       <c r="I3" s="67">
         <f t="shared" ref="I3:I7" si="1">IF(H3&gt;0,H3,0)</f>
-        <v>135.14567999999997</v>
+        <v>125.14567999999997</v>
       </c>
       <c r="J3" s="71">
         <f>I3-I2</f>
@@ -41849,20 +41853,20 @@
         <v>659.43572799999993</v>
       </c>
       <c r="G4" s="74">
-        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B4,Encoding!C:C,C4,Encoding!B:B,'RESULT BALANCE'!D4)</f>
-        <v>-10</v>
+        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B4,Encoding!C:C,C4)</f>
+        <v>-530</v>
       </c>
       <c r="H4" s="80">
         <f t="shared" si="0"/>
-        <v>649.43572799999993</v>
+        <v>129.43572799999993</v>
       </c>
       <c r="I4" s="67">
         <f t="shared" si="1"/>
-        <v>649.43572799999993</v>
+        <v>129.43572799999993</v>
       </c>
       <c r="J4" s="71">
         <f>I4-I3</f>
-        <v>514.29004799999996</v>
+        <v>4.2900479999999561</v>
       </c>
       <c r="M4" s="72"/>
     </row>

</xml_diff>

<commit_message>
issue with first numbers of payment owed
</commit_message>
<xml_diff>
--- a/sofaaudit/input.orig.small.xlsx
+++ b/sofaaudit/input.orig.small.xlsx
@@ -41669,7 +41669,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -41736,20 +41736,20 @@
         <v>560</v>
       </c>
       <c r="G2" s="74">
-        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B2,Encoding!C:C,C2)</f>
-        <v>-530</v>
+        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B2,Encoding!C:C,C2,Encoding!B:B,'RESULT BALANCE'!D2)</f>
+        <v>-520</v>
       </c>
       <c r="H2" s="80">
         <f>G2+F2</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I2" s="67">
         <f>IF(H2&gt;0,H2,0)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J2" s="71">
         <f>I2</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K2" s="67" t="s">
         <v>3655</v>
@@ -41796,16 +41796,16 @@
         <v>655.14567999999997</v>
       </c>
       <c r="G3" s="74">
-        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B3,Encoding!C:C,C3)</f>
-        <v>-530</v>
+        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B3,Encoding!C:C,C3,Encoding!B:B,'RESULT BALANCE'!D3)</f>
+        <v>-520</v>
       </c>
       <c r="H3" s="80">
         <f t="shared" ref="H3:H7" si="0">G3+F3</f>
-        <v>125.14567999999997</v>
+        <v>135.14567999999997</v>
       </c>
       <c r="I3" s="67">
         <f t="shared" ref="I3:I7" si="1">IF(H3&gt;0,H3,0)</f>
-        <v>125.14567999999997</v>
+        <v>135.14567999999997</v>
       </c>
       <c r="J3" s="71">
         <f>I3-I2</f>
@@ -41853,20 +41853,20 @@
         <v>659.43572799999993</v>
       </c>
       <c r="G4" s="74">
-        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B4,Encoding!C:C,C4)</f>
-        <v>-530</v>
+        <f>SUMIFS(Encoding!F:F,Encoding!A:A,'RESULT BALANCE'!B4,Encoding!C:C,C4,Encoding!B:B,'RESULT BALANCE'!D4)</f>
+        <v>-10</v>
       </c>
       <c r="H4" s="80">
         <f t="shared" si="0"/>
-        <v>129.43572799999993</v>
+        <v>649.43572799999993</v>
       </c>
       <c r="I4" s="67">
         <f t="shared" si="1"/>
-        <v>129.43572799999993</v>
+        <v>649.43572799999993</v>
       </c>
       <c r="J4" s="71">
         <f>I4-I3</f>
-        <v>4.2900479999999561</v>
+        <v>514.29004799999996</v>
       </c>
       <c r="M4" s="72"/>
     </row>

</xml_diff>